<commit_message>
Update SHACL and specification files
</commit_message>
<xml_diff>
--- a/01-Dataset1_CV/04-SHACL/Dataset1_CV-Shapes.xlsx
+++ b/01-Dataset1_CV/04-SHACL/Dataset1_CV-Shapes.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\EP\20-Repository\ep-graph-poc\01-Dataset1_CV\04-SHACL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7B7C8E-1A37-47B6-BCA7-CE2F515ED2AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9306B34C-89A9-4F2E-9755-12DDA22468DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26940" windowHeight="13395" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26940" windowHeight="13665" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="119">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -265,13 +265,7 @@
     <t>La liste de code de langues autorisés pour cette valeur</t>
   </si>
   <si>
-    <t>rdf:langString</t>
-  </si>
-  <si>
     <t>sh:node</t>
-  </si>
-  <si>
-    <t>("hu" "et" "fi" "cs" "lk" "lt" "lv" "mt" "en" "da" "nl" "sv" "hr" "sl" "pl" "de" "ro" "it" "pt" "es" "fr" "ga" "el" "bg")</t>
   </si>
   <si>
     <t>epsh:Civility</t>
@@ -382,9 +376,6 @@
     <t>skos:altLabel</t>
   </si>
   <si>
-    <t>rdf:langLiteral</t>
-  </si>
-  <si>
     <t>scheme:Gender</t>
   </si>
   <si>
@@ -422,6 +413,9 @@
   </si>
   <si>
     <t>("en" "fr")</t>
+  </si>
+  <si>
+    <t>("hu" "et" "fi" "cs" "sk" "lt" "lv" "mt" "en" "da" "nl" "sv" "hr" "sl" "pl" "de" "ro" "it" "pt" "es" "fr" "ga" "el" "bg")</t>
   </si>
 </sst>
 </file>
@@ -972,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK21"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1120,17 +1114,17 @@
     </row>
     <row r="9" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1140,7 +1134,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>47</v>
@@ -1151,17 +1145,17 @@
     </row>
     <row r="10" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10"/>
       <c r="D10" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -1171,7 +1165,7 @@
         <v>18</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>47</v>
@@ -1182,17 +1176,17 @@
     </row>
     <row r="11" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1">
         <v>3</v>
@@ -1202,7 +1196,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>47</v>
@@ -1213,17 +1207,17 @@
     </row>
     <row r="12" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="F12" s="1">
         <v>4</v>
@@ -1233,7 +1227,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>47</v>
@@ -1301,9 +1295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN39"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1373,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>55</v>
@@ -1467,7 +1461,7 @@
         <v>31</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="S8" s="9" t="s">
         <v>46</v>
@@ -1476,7 +1470,7 @@
         <v>75</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AMM8"/>
       <c r="AMN8"/>
@@ -1510,7 +1504,7 @@
         <v>38</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>39</v>
@@ -1543,12 +1537,12 @@
         <v>74</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:21 1027:1028" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T10" s="20"/>
     </row>
@@ -1558,10 +1552,10 @@
         <v>epsh:P11</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -1581,7 +1575,7 @@
       </c>
       <c r="Q11" s="1"/>
       <c r="U11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:21 1027:1028" x14ac:dyDescent="0.2">
@@ -1590,10 +1584,10 @@
         <v>epsh:P12</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1608,7 +1602,7 @@
         <v>73</v>
       </c>
       <c r="R12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:21 1027:1028" x14ac:dyDescent="0.2">
@@ -1620,7 +1614,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1642,20 +1636,20 @@
         <v>epsh:P14</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G14"/>
       <c r="L14" t="s">
         <v>44</v>
       </c>
       <c r="M14" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:21 1027:1028" ht="51" x14ac:dyDescent="0.2">
@@ -1667,7 +1661,7 @@
         <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -1676,13 +1670,13 @@
         <v>44</v>
       </c>
       <c r="M15" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="S15" t="s">
         <v>47</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:21 1027:1028" x14ac:dyDescent="0.2">
@@ -1690,7 +1684,7 @@
     </row>
     <row r="18" spans="1:21" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T18" s="20"/>
     </row>
@@ -1700,10 +1694,10 @@
         <v>epsh:P19</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
         <v>43</v>
@@ -1723,7 +1717,7 @@
       </c>
       <c r="Q19" s="1"/>
       <c r="U19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -1735,7 +1729,7 @@
         <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1756,10 +1750,10 @@
         <v>epsh:P21</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1783,7 +1777,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1807,7 +1801,7 @@
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G23">
         <v>24</v>
@@ -1819,18 +1813,18 @@
         <v>44</v>
       </c>
       <c r="M23" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="S23" t="s">
         <v>47</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="T25" s="20"/>
     </row>
@@ -1840,10 +1834,10 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -1863,7 +1857,7 @@
       </c>
       <c r="Q26" s="1"/>
       <c r="U26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
@@ -1875,7 +1869,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G27" s="1">
         <v>1</v>
@@ -1896,10 +1890,10 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -1911,7 +1905,7 @@
         <v>44</v>
       </c>
       <c r="M28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
@@ -1920,10 +1914,10 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -1935,7 +1929,7 @@
         <v>44</v>
       </c>
       <c r="M29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
@@ -1944,10 +1938,10 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1965,10 +1959,10 @@
         <v>epsh:P31</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1986,10 +1980,10 @@
         <v>epsh:P32</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -2004,7 +1998,7 @@
         <v>73</v>
       </c>
       <c r="R32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,10 +2007,10 @@
         <v>epsh:P33</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -2040,7 +2034,7 @@
         <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G34">
         <v>24</v>
@@ -2052,13 +2046,13 @@
         <v>44</v>
       </c>
       <c r="M34" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="S34" t="s">
         <v>47</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -2067,10 +2061,10 @@
         <v>epsh:P35</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G35">
         <v>24</v>
@@ -2082,15 +2076,15 @@
         <v>44</v>
       </c>
       <c r="M35" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T36" s="20"/>
     </row>
@@ -2100,10 +2094,10 @@
         <v>epsh:P37</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
         <v>43</v>
@@ -2123,7 +2117,7 @@
       </c>
       <c r="Q37" s="1"/>
       <c r="U37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
@@ -2135,7 +2129,7 @@
         <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -2159,7 +2153,7 @@
         <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G39" s="1">
         <v>1</v>
@@ -2171,13 +2165,13 @@
         <v>44</v>
       </c>
       <c r="M39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="S39" t="s">
         <v>47</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update plainLiterals -> xsd:string
</commit_message>
<xml_diff>
--- a/01-Dataset1_CV/04-SHACL/Dataset1_CV-Shapes.xlsx
+++ b/01-Dataset1_CV/04-SHACL/Dataset1_CV-Shapes.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\EP\20-Repository\ep-graph-poc\01-Dataset1_CV\04-SHACL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9306B34C-89A9-4F2E-9755-12DDA22468DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A90BD8C-2665-4BA8-A88B-2EB44D11E4B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26940" windowHeight="13665" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="120">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>xsd:integer</t>
-  </si>
-  <si>
-    <t>rdf:plainLiteral</t>
   </si>
   <si>
     <t>sh:languageIn</t>
@@ -416,6 +413,12 @@
   </si>
   <si>
     <t>("hu" "et" "fi" "cs" "sk" "lt" "lv" "mt" "en" "da" "nl" "sv" "hr" "sl" "pl" "de" "ro" "it" "pt" "es" "fr" "ga" "el" "bg")</t>
+  </si>
+  <si>
+    <t>xsd:string</t>
+  </si>
+  <si>
+    <t>rdf:langString</t>
   </si>
 </sst>
 </file>
@@ -1114,17 +1117,17 @@
     </row>
     <row r="9" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1134,7 +1137,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>47</v>
@@ -1145,17 +1148,17 @@
     </row>
     <row r="10" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10"/>
       <c r="D10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -1165,7 +1168,7 @@
         <v>18</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>47</v>
@@ -1176,17 +1179,17 @@
     </row>
     <row r="11" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="F11" s="1">
         <v>3</v>
@@ -1196,7 +1199,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>47</v>
@@ -1207,17 +1210,17 @@
     </row>
     <row r="12" spans="1:11 1025:1025" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="1">
         <v>4</v>
@@ -1227,7 +1230,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>47</v>
@@ -1295,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN39"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
@@ -1367,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>55</v>
@@ -1461,16 +1464,16 @@
         <v>31</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S8" s="9" t="s">
         <v>46</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AMM8"/>
       <c r="AMN8"/>
@@ -1504,7 +1507,7 @@
         <v>38</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>39</v>
@@ -1534,15 +1537,15 @@
         <v>45</v>
       </c>
       <c r="T9" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:21 1027:1028" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T10" s="20"/>
     </row>
@@ -1552,10 +1555,10 @@
         <v>epsh:P11</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -1575,7 +1578,7 @@
       </c>
       <c r="Q11" s="1"/>
       <c r="U11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:21 1027:1028" x14ac:dyDescent="0.2">
@@ -1584,10 +1587,10 @@
         <v>epsh:P12</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1599,10 +1602,10 @@
         <v>44</v>
       </c>
       <c r="M12" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="R12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:21 1027:1028" x14ac:dyDescent="0.2">
@@ -1614,7 +1617,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1626,7 +1629,7 @@
         <v>44</v>
       </c>
       <c r="M13" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="R13" s="13"/>
     </row>
@@ -1636,20 +1639,20 @@
         <v>epsh:P14</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14"/>
       <c r="L14" t="s">
         <v>44</v>
       </c>
       <c r="M14" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:21 1027:1028" ht="51" x14ac:dyDescent="0.2">
@@ -1661,7 +1664,7 @@
         <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -1670,13 +1673,13 @@
         <v>44</v>
       </c>
       <c r="M15" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="S15" t="s">
         <v>47</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:21 1027:1028" x14ac:dyDescent="0.2">
@@ -1684,7 +1687,7 @@
     </row>
     <row r="18" spans="1:21" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T18" s="20"/>
     </row>
@@ -1694,10 +1697,10 @@
         <v>epsh:P19</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
         <v>43</v>
@@ -1717,7 +1720,7 @@
       </c>
       <c r="Q19" s="1"/>
       <c r="U19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -1729,7 +1732,7 @@
         <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1741,7 +1744,7 @@
         <v>44</v>
       </c>
       <c r="M20" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -1750,10 +1753,10 @@
         <v>epsh:P21</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1765,7 +1768,7 @@
         <v>44</v>
       </c>
       <c r="M21" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
@@ -1777,7 +1780,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1789,7 +1792,7 @@
         <v>44</v>
       </c>
       <c r="M22" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -1801,7 +1804,7 @@
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G23">
         <v>24</v>
@@ -1813,18 +1816,18 @@
         <v>44</v>
       </c>
       <c r="M23" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="S23" t="s">
         <v>47</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T25" s="20"/>
     </row>
@@ -1834,10 +1837,10 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -1857,7 +1860,7 @@
       </c>
       <c r="Q26" s="1"/>
       <c r="U26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
@@ -1869,7 +1872,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" s="1">
         <v>1</v>
@@ -1881,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="M27" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
@@ -1890,10 +1893,10 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -1905,7 +1908,7 @@
         <v>44</v>
       </c>
       <c r="M28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
@@ -1914,10 +1917,10 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -1929,7 +1932,7 @@
         <v>44</v>
       </c>
       <c r="M29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
@@ -1938,10 +1941,10 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1959,10 +1962,10 @@
         <v>epsh:P31</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1980,10 +1983,10 @@
         <v>epsh:P32</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -1995,10 +1998,10 @@
         <v>44</v>
       </c>
       <c r="M32" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="R32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2007,10 +2010,10 @@
         <v>epsh:P33</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -2034,7 +2037,7 @@
         <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34">
         <v>24</v>
@@ -2046,13 +2049,13 @@
         <v>44</v>
       </c>
       <c r="M34" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="S34" t="s">
         <v>47</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -2061,10 +2064,10 @@
         <v>epsh:P35</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G35">
         <v>24</v>
@@ -2076,15 +2079,15 @@
         <v>44</v>
       </c>
       <c r="M35" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T36" s="20"/>
     </row>
@@ -2094,10 +2097,10 @@
         <v>epsh:P37</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
         <v>43</v>
@@ -2117,7 +2120,7 @@
       </c>
       <c r="Q37" s="1"/>
       <c r="U37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
@@ -2129,7 +2132,7 @@
         <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -2141,7 +2144,7 @@
         <v>44</v>
       </c>
       <c r="M38" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
@@ -2153,7 +2156,7 @@
         <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G39" s="1">
         <v>1</v>
@@ -2165,13 +2168,13 @@
         <v>44</v>
       </c>
       <c r="M39" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="S39" t="s">
         <v>47</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update eponto namespace and adjusted some stuff
</commit_message>
<xml_diff>
--- a/01-Dataset1_CV/04-SHACL/Dataset1_CV-Shapes.xlsx
+++ b/01-Dataset1_CV/04-SHACL/Dataset1_CV-Shapes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">eponto</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.europa.eu/ontology/ep#</t>
+    <t xml:space="preserve">http://data.europarl.europa.eu/ontology/ep#</t>
   </si>
   <si>
     <t xml:space="preserve">Cette feuille spécifie la liste de Shapes basées sur des classes</t>
@@ -128,34 +128,7 @@
     <t xml:space="preserve">sh:IRI</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/civility/.*$</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/civility/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">true</t>
@@ -173,34 +146,7 @@
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/gender/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/gender/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:Country</t>
@@ -212,34 +158,7 @@
     <t xml:space="preserve">Country</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/country/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/country/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:ConceptStatus</t>
@@ -251,34 +170,7 @@
     <t xml:space="preserve">Concept Status</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/conceptStatus/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/conceptStatus/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">scheme</t>
@@ -677,14 +569,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -725,12 +617,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -833,11 +725,11 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -846,7 +738,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="53.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.57"/>
@@ -867,11 +759,11 @@
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -880,11 +772,11 @@
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -893,21 +785,21 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="3"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -1009,7 +901,7 @@
       <c r="H11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="15" t="s">
         <v>35</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1040,7 +932,7 @@
       <c r="H12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="15" t="s">
         <v>41</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1071,7 +963,7 @@
       <c r="H13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="15" t="s">
         <v>45</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -1102,7 +994,7 @@
       <c r="H14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="15" t="s">
         <v>49</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -1113,10 +1005,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="15"/>
+      <c r="D15" s="16"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
@@ -1151,10 +1043,10 @@
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes"/>
     <hyperlink ref="E10" r:id="rId2" display="rdfs:label@fr"/>
     <hyperlink ref="G10" r:id="rId3" display="rdfs:comment@fr"/>
-    <hyperlink ref="I11" r:id="rId4" display="http://data.europarl.europa.eu/authority/civility/.*$"/>
-    <hyperlink ref="I12" r:id="rId5" display="http://data.europarl.europa.eu/authority/gender/"/>
-    <hyperlink ref="I13" r:id="rId6" display="http://data.europarl.europa.eu/authority/country/"/>
-    <hyperlink ref="I14" r:id="rId7" display="http://data.europarl.europa.eu/authority/conceptStatus/"/>
+    <hyperlink ref="I11" r:id="rId4" display="&quot;^http://data.europarl.europa.eu/authority/civility/.*$&quot;"/>
+    <hyperlink ref="I12" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/authority/gender/.*$&quot;"/>
+    <hyperlink ref="I13" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/authority/country/.*$&quot;"/>
+    <hyperlink ref="I14" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/authority/conceptStatus/.*$&quot;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1173,21 +1065,21 @@
   </sheetPr>
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="T17" activeCellId="0" sqref="T17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="U39" activeCellId="0" sqref="U39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.42"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.14"/>
@@ -1216,7 +1108,7 @@
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="1"/>
@@ -1228,7 +1120,7 @@
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="Q3" s="1"/>
@@ -1240,7 +1132,7 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1252,13 +1144,13 @@
       <c r="B5" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -1283,7 +1175,7 @@
       <c r="R7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G8" s="4"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" s="11" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
@@ -1503,7 +1395,7 @@
       <c r="M14" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="R14" s="16"/>
+      <c r="R14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
@@ -1573,7 +1465,7 @@
       <c r="Q17" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="R17" s="16"/>
+      <c r="R17" s="15"/>
     </row>
     <row r="19" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">

</xml_diff>